<commit_message>
created skeleton lakeidGenerator and added S3 key integration (S3 not integrated yet, just defined the keys in index.py)
</commit_message>
<xml_diff>
--- a/assets/GLEON_GMA_Example.xlsx
+++ b/assets/GLEON_GMA_Example.xlsx
@@ -1,17 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hredwards/Desktop/DataScience Job/ThisisIt/assets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB26B7F-B068-D54C-A2EC-4E66E8A9D009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14020"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="29860" windowHeight="21840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GLEON_GMA_Example csv" sheetId="1" r:id="rId1"/>
-    <sheet name="Description" sheetId="2" r:id="rId2"/>
+    <sheet name="Column Comparison" sheetId="3" r:id="rId2"/>
+    <sheet name="Description" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="149">
   <si>
     <t>Date</t>
   </si>
@@ -401,13 +416,79 @@
   </si>
   <si>
     <t>Dataset_ID</t>
+  </si>
+  <si>
+    <t>CSV Columns</t>
+  </si>
+  <si>
+    <t>Excel Columns</t>
+  </si>
+  <si>
+    <t>Microcystin</t>
+  </si>
+  <si>
+    <t>Anatoxin-a</t>
+  </si>
+  <si>
+    <t>Cylindrospermopsin</t>
+  </si>
+  <si>
+    <t>Saxitoxin</t>
+  </si>
+  <si>
+    <t>Nodularin</t>
+  </si>
+  <si>
+    <t>Geosmin</t>
+  </si>
+  <si>
+    <t>2-MIB</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>Secchi</t>
+  </si>
+  <si>
+    <t>Chl</t>
+  </si>
+  <si>
+    <t>NO2+3</t>
+  </si>
+  <si>
+    <t>NO3</t>
+  </si>
+  <si>
+    <t>NH3</t>
+  </si>
+  <si>
+    <t>OrthoP</t>
+  </si>
+  <si>
+    <t>SRP</t>
+  </si>
+  <si>
+    <t>TotalPhytoCells</t>
+  </si>
+  <si>
+    <t>CyanobacterialCells</t>
+  </si>
+  <si>
+    <t>mcyDgeneAbund</t>
+  </si>
+  <si>
+    <t>mcyEgeneAbund</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1410,21 +1491,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -1625,21 +1706,395 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A1DC08-3225-B442-BF52-3EE2B9BFCB67}">
+  <dimension ref="A1:B55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="72.6640625" customWidth="1"/>
     <col min="3" max="3" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1">
+    <row r="1" spans="1:3" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
@@ -1650,7 +2105,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1">
+    <row r="2" spans="1:3" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>126</v>
       </c>
@@ -1661,7 +2116,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1">
+    <row r="3" spans="1:3" ht="16" thickBot="1">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1672,7 +2127,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1">
+    <row r="4" spans="1:3" ht="16" thickBot="1">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1683,7 +2138,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1">
+    <row r="5" spans="1:3" ht="16" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>106</v>
       </c>
@@ -1694,7 +2149,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1">
+    <row r="6" spans="1:3" ht="16" thickBot="1">
       <c r="A6" s="9" t="s">
         <v>60</v>
       </c>
@@ -1705,7 +2160,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1">
+    <row r="7" spans="1:3" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1716,7 +2171,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1">
+    <row r="8" spans="1:3" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
@@ -1727,7 +2182,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1">
+    <row r="9" spans="1:3" ht="16" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1738,7 +2193,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1">
+    <row r="10" spans="1:3" ht="16" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1749,7 +2204,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1">
+    <row r="11" spans="1:3" ht="16" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1760,7 +2215,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1">
+    <row r="12" spans="1:3" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1771,7 +2226,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1">
+    <row r="13" spans="1:3" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
@@ -1782,7 +2237,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="25" thickBot="1">
+    <row r="14" spans="1:3" ht="29" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -1793,7 +2248,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1">
+    <row r="15" spans="1:3" ht="16" thickBot="1">
       <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
@@ -1804,7 +2259,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1">
+    <row r="16" spans="1:3" ht="16" thickBot="1">
       <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
@@ -1815,7 +2270,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
+    <row r="17" spans="1:3" ht="16" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
@@ -1826,7 +2281,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1">
+    <row r="18" spans="1:3" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>16</v>
       </c>
@@ -1837,7 +2292,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1">
+    <row r="19" spans="1:3" ht="16" thickBot="1">
       <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
@@ -1848,7 +2303,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1">
+    <row r="20" spans="1:3" ht="16" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>19</v>
       </c>
@@ -1859,7 +2314,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1">
+    <row r="21" spans="1:3" ht="16" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>20</v>
       </c>
@@ -1870,7 +2325,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1">
+    <row r="22" spans="1:3" ht="16" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>21</v>
       </c>
@@ -1881,7 +2336,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1">
+    <row r="23" spans="1:3" ht="16" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>22</v>
       </c>
@@ -1892,7 +2347,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1">
+    <row r="24" spans="1:3" ht="16" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>23</v>
       </c>
@@ -1903,7 +2358,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1">
+    <row r="25" spans="1:3" ht="16" thickBot="1">
       <c r="A25" s="9" t="s">
         <v>24</v>
       </c>
@@ -1914,7 +2369,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1">
+    <row r="26" spans="1:3" ht="16" thickBot="1">
       <c r="A26" s="9" t="s">
         <v>25</v>
       </c>
@@ -1925,7 +2380,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1">
+    <row r="27" spans="1:3" ht="16" thickBot="1">
       <c r="A27" s="9" t="s">
         <v>26</v>
       </c>
@@ -1936,7 +2391,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1">
+    <row r="28" spans="1:3" ht="16" thickBot="1">
       <c r="A28" s="9" t="s">
         <v>27</v>
       </c>
@@ -1947,7 +2402,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1">
+    <row r="29" spans="1:3" ht="16" thickBot="1">
       <c r="A29" s="9" t="s">
         <v>28</v>
       </c>
@@ -1958,7 +2413,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1">
+    <row r="30" spans="1:3" ht="16" thickBot="1">
       <c r="A30" s="9" t="s">
         <v>29</v>
       </c>
@@ -1969,7 +2424,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1">
+    <row r="31" spans="1:3" ht="16" thickBot="1">
       <c r="A31" s="9" t="s">
         <v>30</v>
       </c>
@@ -1980,7 +2435,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1">
+    <row r="32" spans="1:3" ht="16" thickBot="1">
       <c r="A32" s="9" t="s">
         <v>31</v>
       </c>
@@ -1991,7 +2446,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1">
+    <row r="33" spans="1:3" ht="16" thickBot="1">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -2002,7 +2457,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1">
+    <row r="34" spans="1:3" ht="16" thickBot="1">
       <c r="A34" s="9" t="s">
         <v>110</v>
       </c>
@@ -2013,7 +2468,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1">
+    <row r="35" spans="1:3" ht="16" thickBot="1">
       <c r="A35" s="9" t="s">
         <v>124</v>
       </c>
@@ -2024,7 +2479,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1">
+    <row r="36" spans="1:3" ht="16" thickBot="1">
       <c r="A36" s="9" t="s">
         <v>36</v>
       </c>
@@ -2035,7 +2490,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" thickBot="1">
+    <row r="37" spans="1:3" ht="16" thickBot="1">
       <c r="A37" s="9" t="s">
         <v>35</v>
       </c>
@@ -2046,7 +2501,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1">
+    <row r="38" spans="1:3" ht="16" thickBot="1">
       <c r="A38" s="9" t="s">
         <v>34</v>
       </c>
@@ -2057,7 +2512,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" thickBot="1">
+    <row r="39" spans="1:3" ht="16" thickBot="1">
       <c r="A39" s="9" t="s">
         <v>37</v>
       </c>
@@ -2068,7 +2523,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1">
+    <row r="40" spans="1:3" ht="16" thickBot="1">
       <c r="A40" s="9" t="s">
         <v>38</v>
       </c>
@@ -2079,7 +2534,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" thickBot="1">
+    <row r="41" spans="1:3" ht="16" thickBot="1">
       <c r="A41" s="9" t="s">
         <v>39</v>
       </c>
@@ -2090,7 +2545,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1">
+    <row r="42" spans="1:3" ht="16" thickBot="1">
       <c r="A42" s="9" t="s">
         <v>40</v>
       </c>
@@ -2101,7 +2556,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1">
+    <row r="43" spans="1:3" ht="16" thickBot="1">
       <c r="A43" s="9" t="s">
         <v>41</v>
       </c>
@@ -2112,7 +2567,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1">
+    <row r="44" spans="1:3" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>42</v>
       </c>
@@ -2123,7 +2578,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15" thickBot="1">
+    <row r="45" spans="1:3" ht="16" thickBot="1">
       <c r="A45" s="9" t="s">
         <v>43</v>
       </c>
@@ -2134,7 +2589,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1">
+    <row r="46" spans="1:3" ht="16" thickBot="1">
       <c r="A46" s="11" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
upload now sends to AWS folder; added filtered graphs page (not functioning properly yet); cleaned up graphs layout on homepage
</commit_message>
<xml_diff>
--- a/assets/GLEON_GMA_Example.xlsx
+++ b/assets/GLEON_GMA_Example.xlsx
@@ -1,32 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hredwards/Desktop/DataScience Job/ThisisIt/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hredwards/Desktop/Desktop - Hallie's Mac Pro/DataScience Job/Environmental Science Projects and Data/Original Data Set and Dash/GLEON-GMA-master/dash/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB26B7F-B068-D54C-A2EC-4E66E8A9D009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DF4247-D6F9-2243-8C14-014178FCA8BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="29860" windowHeight="21840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GLEON_GMA_Example csv" sheetId="1" r:id="rId1"/>
-    <sheet name="Column Comparison" sheetId="3" r:id="rId2"/>
-    <sheet name="Description" sheetId="2" r:id="rId3"/>
+    <sheet name="Description" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -35,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="127">
   <si>
     <t>Date</t>
   </si>
@@ -416,72 +407,6 @@
   </si>
   <si>
     <t>Dataset_ID</t>
-  </si>
-  <si>
-    <t>CSV Columns</t>
-  </si>
-  <si>
-    <t>Excel Columns</t>
-  </si>
-  <si>
-    <t>Microcystin</t>
-  </si>
-  <si>
-    <t>Anatoxin-a</t>
-  </si>
-  <si>
-    <t>Cylindrospermopsin</t>
-  </si>
-  <si>
-    <t>Saxitoxin</t>
-  </si>
-  <si>
-    <t>Nodularin</t>
-  </si>
-  <si>
-    <t>Geosmin</t>
-  </si>
-  <si>
-    <t>2-MIB</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>TP</t>
-  </si>
-  <si>
-    <t>Secchi</t>
-  </si>
-  <si>
-    <t>Chl</t>
-  </si>
-  <si>
-    <t>NO2+3</t>
-  </si>
-  <si>
-    <t>NO3</t>
-  </si>
-  <si>
-    <t>NH3</t>
-  </si>
-  <si>
-    <t>OrthoP</t>
-  </si>
-  <si>
-    <t>SRP</t>
-  </si>
-  <si>
-    <t>TotalPhytoCells</t>
-  </si>
-  <si>
-    <t>CyanobacterialCells</t>
-  </si>
-  <si>
-    <t>mcyDgeneAbund</t>
-  </si>
-  <si>
-    <t>mcyEgeneAbund</t>
   </si>
 </sst>
 </file>
@@ -1501,9 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -1706,384 +1629,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A1DC08-3225-B442-BF52-3EE2B9BFCB67}">
-  <dimension ref="A1:B55"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>147</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="B28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="B29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="B30" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="B31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="B32" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>